<commit_message>
Agrego archivos a la carpeta
</commit_message>
<xml_diff>
--- a/Casos-de-uso.xlsx
+++ b/Casos-de-uso.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="14115" windowHeight="4680" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="15480" windowHeight="11205" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
   <si>
     <t>Nro de Caso de Uso</t>
   </si>
@@ -301,9 +301,6 @@
     <t>Modifica una habitacion</t>
   </si>
   <si>
-    <t>Ingresa al sistema un tipo de usuario: encargado, recepcionista</t>
-  </si>
-  <si>
     <t>Saca del sistema un tipo de usuario</t>
   </si>
   <si>
@@ -314,13 +311,46 @@
   </si>
   <si>
     <t>Salida del cliente</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>No veo la forma de asociar un ticket a un cliente sin que este tenga una estadia, podriamos agregar tickets al cliente?</t>
+  </si>
+  <si>
+    <t>La lista de servicios deberia estar en la estadia</t>
+  </si>
+  <si>
+    <t>Como resolveriamos el tema de marcar cuando una habitacion esta ocupada o esta libre</t>
+  </si>
+  <si>
+    <t>Mismo problema de asociacion entre cliente y ticket</t>
+  </si>
+  <si>
+    <t>Faltaria en el diagrama una entidad que represente</t>
+  </si>
+  <si>
+    <t>Se agregaria a la estadia, por eso es que falta la lista de servicios</t>
+  </si>
+  <si>
+    <t>Tabla tareas pendientes???</t>
+  </si>
+  <si>
+    <t>Idem</t>
+  </si>
+  <si>
+    <t>Tabla ofertas? Como las cargamos(podria ser una pantalla para el admin)?</t>
+  </si>
+  <si>
+    <t>Ingresa al sistema un tipo de usuario: encargado, recepcionista,cliente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,7 +470,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -475,7 +504,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -651,14 +679,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
@@ -666,7 +694,7 @@
     <col min="5" max="5" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -694,7 +722,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -708,7 +736,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -722,7 +750,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -736,7 +764,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -749,8 +777,11 @@
       <c r="D6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -764,7 +795,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -777,8 +808,11 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -792,7 +826,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -805,8 +839,11 @@
       <c r="D10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -819,8 +856,11 @@
       <c r="D11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -840,14 +880,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
@@ -855,7 +895,7 @@
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -869,7 +909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -883,7 +923,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -897,7 +937,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -911,7 +951,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -925,7 +965,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -939,7 +979,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -953,7 +993,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -967,7 +1007,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -980,8 +1020,11 @@
       <c r="D9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -994,8 +1037,11 @@
       <c r="D10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1009,7 +1055,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1023,7 +1069,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1037,7 +1083,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1051,7 +1097,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1065,7 +1111,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1079,7 +1125,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1090,10 +1136,10 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1105,6 +1151,9 @@
       </c>
       <c r="D18" t="s">
         <v>71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1113,21 +1162,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
     <col min="5" max="5" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1154,8 +1203,11 @@
       <c r="D2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1168,8 +1220,11 @@
       <c r="D3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1183,7 +1238,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1197,7 +1252,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1211,7 +1266,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1231,21 +1286,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" customWidth="1"/>
     <col min="4" max="5" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1259,7 +1314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1272,8 +1327,11 @@
       <c r="D2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1284,10 +1342,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1298,10 +1356,10 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1315,7 +1373,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1329,7 +1387,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1343,7 +1401,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1357,7 +1415,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1371,7 +1429,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1385,7 +1443,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1399,7 +1457,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1413,7 +1471,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1424,10 +1482,10 @@
         <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1438,10 +1496,10 @@
         <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1452,7 +1510,7 @@
         <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>